<commit_message>
removed the browser() in CapQuery.R and tried out a logic in RYG.R
</commit_message>
<xml_diff>
--- a/Dashboard/FCA_RYG.xlsx
+++ b/Dashboard/FCA_RYG.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9396"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,9 +56,6 @@
     <t>C_PMSC_ev_PT_SignHtrMin</t>
   </si>
   <si>
-    <t xml:space="preserve">P_PMSC_PT_IntgAbsExhAccel            </t>
-  </si>
-  <si>
     <t>None</t>
   </si>
   <si>
@@ -156,13 +153,16 @@
   </si>
   <si>
     <t>&gt; -2.5</t>
+  </si>
+  <si>
+    <t>P_PMSC_PT_IntgAbsExhAccel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,6 +173,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -198,11 +206,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -486,7 +495,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -498,30 +507,30 @@
     <col min="7" max="7" width="28.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -545,7 +554,7 @@
       </c>
       <c r="G2" s="1"/>
       <c r="H2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -559,16 +568,16 @@
         <v>6</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>11</v>
       </c>
-      <c r="G3" t="s">
-        <v>12</v>
-      </c>
       <c r="H3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -582,16 +591,16 @@
         <v>6</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="H4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -602,19 +611,19 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
         <v>19</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>20</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>21</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>22</v>
-      </c>
-      <c r="H5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -625,19 +634,19 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" t="s">
         <v>27</v>
-      </c>
-      <c r="D6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -645,22 +654,22 @@
         <v>13096</v>
       </c>
       <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" t="s">
         <v>32</v>
-      </c>
-      <c r="C7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="H7" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -671,19 +680,19 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="H8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -694,19 +703,19 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="H9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -717,19 +726,19 @@
         <v>0</v>
       </c>
       <c r="C10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E10" t="s">
-        <v>21</v>
-      </c>
-      <c r="G10" s="1" t="s">
+      <c r="H10" t="s">
         <v>42</v>
-      </c>
-      <c r="H10" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>